<commit_message>
update peptide-based analysis (version 2)
Updated the codes and files of three datasets (mainly replaced MSqRob with msqrob2)
</commit_message>
<xml_diff>
--- a/r-research/based-peptide-analysis/PXD000279/msqrob-quantms_experimental_annotation.xlsx
+++ b/r-research/based-peptide-analysis/PXD000279/msqrob-quantms_experimental_annotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dataset\R downstream analysis\0-paper\data_benchmark\0-reviewer\peptide based\PXD000279\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798FC9ED-1DE3-4E9C-B469-F2DBF4F0E285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B2CAF6-8FB6-4CCF-B648-EDE2FA1CC4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="1095" windowWidth="22140" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="22140" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -25,31 +25,6 @@
     <t>run</t>
   </si>
   <si>
-    <t>peptide_abundance_study_variable.2.</t>
-  </si>
-  <si>
-    <t>peptide_abundance_study_variable.3.</t>
-  </si>
-  <si>
-    <t>peptide_abundance_study_variable.4.</t>
-  </si>
-  <si>
-    <t>peptide_abundance_study_variable.5.</t>
-  </si>
-  <si>
-    <t>peptide_abundance_study_variable.6.</t>
-  </si>
-  <si>
-    <t>peptide_abundance_study_variable.7.</t>
-  </si>
-  <si>
-    <t>peptide_abundance_study_variable.8.</t>
-  </si>
-  <si>
-    <t>peptide_abundance_study_variable.1.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>treatment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -60,6 +35,31 @@
   <si>
     <t>UPS2</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sumIntensity_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sumIntensity_2</t>
+  </si>
+  <si>
+    <t>sumIntensity_3</t>
+  </si>
+  <si>
+    <t>sumIntensity_4</t>
+  </si>
+  <si>
+    <t>sumIntensity_5</t>
+  </si>
+  <si>
+    <t>sumIntensity_6</t>
+  </si>
+  <si>
+    <t>sumIntensity_7</t>
+  </si>
+  <si>
+    <t>sumIntensity_8</t>
   </si>
 </sst>
 </file>
@@ -403,81 +403,84 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>